<commit_message>
Comentários todos em ingles, parâmetros dos dados de entrada, e revisão do codigo
</commit_message>
<xml_diff>
--- a/Input Data - Other.xlsx
+++ b/Input Data - Other.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugo.serrano\PycharmProjects1\CREATE VALLEY T4.3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugo.serrano\PycharmProjects1\CRETE_VALLEY_T.4.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA19F898-B1A5-4B14-A337-3008DB6E2176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84AEDE6-1BB3-40C7-882C-19200E563DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5973E1B4-7AE7-44FD-A290-C7CC6048C959}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5973E1B4-7AE7-44FD-A290-C7CC6048C959}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather forecasts" sheetId="2" r:id="rId1"/>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C0EE47-0B50-41E0-A581-86A0AF2BDC0A}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,13 +672,13 @@
         <v>0.45400000000000001</v>
       </c>
       <c r="M2" s="1">
-        <v>0.51300000000000001</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="N2" s="1">
-        <v>0.57199999999999995</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="O2" s="1">
-        <v>0.46500000000000002</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="P2" s="1">
         <v>0.52100000000000002</v>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4891DC18-5D0D-41C4-B0B2-538456E33E75}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y23" sqref="Y23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1597,16 +1597,16 @@
         <v>75</v>
       </c>
       <c r="G11" s="3">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H11" s="3">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="I11" s="3">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J11" s="3">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="K11" s="3">
         <v>80</v>

</xml_diff>

<commit_message>
Atualização dos arquivos de entrada Excel
</commit_message>
<xml_diff>
--- a/Input Data - Other.xlsx
+++ b/Input Data - Other.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugo.serrano\PycharmProjects1\CRETE_VALLEY_T.4.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84AEDE6-1BB3-40C7-882C-19200E563DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B23D84-9194-4460-B19D-D96D4D210743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5973E1B4-7AE7-44FD-A290-C7CC6048C959}"/>
+    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5973E1B4-7AE7-44FD-A290-C7CC6048C959}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather forecasts" sheetId="2" r:id="rId1"/>
@@ -798,7 +798,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:J11"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1588,13 +1588,13 @@
         <v>75</v>
       </c>
       <c r="D11" s="3">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F11" s="3">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G11" s="3">
         <v>75</v>

</xml_diff>